<commit_message>
organize the cards by suit then rank
</commit_message>
<xml_diff>
--- a/card_data/D/des-philosophes-de-lan.xlsx
+++ b/card_data/D/des-philosophes-de-lan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alyssa/Documents/GitHub/playing-cards/backend/app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\dhmit\french-playing-cards\card_data\D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED70F6A9-9ECA-6044-B068-73918AF6C5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ABB938-0F3D-4912-ADFE-F9F00C7F9754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="1000" windowWidth="27640" windowHeight="15960" xr2:uid="{71E25E93-68D8-F447-AD35-34F8AFF9FFBB}"/>
+    <workbookView xWindow="-20840" yWindow="-10000" windowWidth="16200" windowHeight="28510" xr2:uid="{71E25E93-68D8-F447-AD35-34F8AFF9FFBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="37">
   <si>
     <t>DB ID</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>des_philosophes_de_lan.JS.1</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -516,15 +528,15 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="28.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -572,7 +584,9 @@
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
@@ -596,7 +610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -606,7 +620,9 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
@@ -630,7 +646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -640,7 +656,9 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
@@ -664,7 +682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -674,7 +692,9 @@
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
@@ -698,7 +718,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -708,7 +728,9 @@
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
@@ -732,7 +754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -742,7 +764,9 @@
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
@@ -766,7 +790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -776,7 +800,9 @@
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
@@ -800,7 +826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -810,7 +836,9 @@
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
@@ -834,7 +862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -844,7 +872,9 @@
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
@@ -868,7 +898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -878,7 +908,9 @@
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
@@ -902,7 +934,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -912,7 +944,9 @@
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>12</v>
       </c>
@@ -936,7 +970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -946,7 +980,9 @@
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
clean up card model, don't show backs when theyd on't exist
</commit_message>
<xml_diff>
--- a/card_data/D/des-philosophes-de-lan.xlsx
+++ b/card_data/D/des-philosophes-de-lan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\dhmit\french-playing-cards\card_data\D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ABB938-0F3D-4912-ADFE-F9F00C7F9754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5900CAE-5FD3-4B91-BF4B-800B438C51F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20840" yWindow="-10000" windowWidth="16200" windowHeight="28510" xr2:uid="{71E25E93-68D8-F447-AD35-34F8AFF9FFBB}"/>
+    <workbookView xWindow="4990" yWindow="1210" windowWidth="23260" windowHeight="24650" xr2:uid="{71E25E93-68D8-F447-AD35-34F8AFF9FFBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -528,7 +528,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>